<commit_message>
Page Load Performance- Completed
</commit_message>
<xml_diff>
--- a/WSI_MCP_TestData.xlsx
+++ b/WSI_MCP_TestData.xlsx
@@ -4,22 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="6840" activeTab="5"/>
+    <workbookView windowWidth="19200" windowHeight="7110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ManageAttributes" sheetId="1" r:id="rId1"/>
     <sheet name="ManageSeason" sheetId="2" r:id="rId2"/>
     <sheet name="Libraries" sheetId="4" r:id="rId3"/>
-    <sheet name="ManageTypes" sheetId="5" r:id="rId4"/>
-    <sheet name="FilterHeader" sheetId="6" r:id="rId5"/>
-    <sheet name="LDAPRoles" sheetId="7" r:id="rId6"/>
+    <sheet name="FilterHeader" sheetId="6" r:id="rId4"/>
+    <sheet name="LDAPRoles" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="335">
   <si>
     <t>DataType</t>
   </si>
@@ -444,19 +443,49 @@
     <t>SubMenu</t>
   </si>
   <si>
+    <t>Division</t>
+  </si>
+  <si>
     <t>Country</t>
   </si>
   <si>
     <t>Vendor</t>
   </si>
   <si>
+    <t>Lading Port</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Season Collection</t>
+  </si>
+  <si>
+    <t>Diffs</t>
+  </si>
+  <si>
+    <t>Diff Material</t>
+  </si>
+  <si>
+    <t>JDA Hierarchy</t>
+  </si>
+  <si>
+    <t>Business Objects</t>
+  </si>
+  <si>
+    <t>Royalty</t>
+  </si>
+  <si>
     <t>Item</t>
   </si>
   <si>
+    <t>Tabletop</t>
+  </si>
+  <si>
     <t>Item-Pack-Components</t>
   </si>
   <si>
-    <t>Agent</t>
+    <t>Textiles</t>
   </si>
   <si>
     <t>Item-Season</t>
@@ -465,21 +494,9 @@
     <t>Item-Parent-Season</t>
   </si>
   <si>
-    <t>Lading Port</t>
-  </si>
-  <si>
-    <t>JDA Hierarchy</t>
-  </si>
-  <si>
     <t>Merch Hierarchy</t>
   </si>
   <si>
-    <t>Diffs</t>
-  </si>
-  <si>
-    <t>Business Objects</t>
-  </si>
-  <si>
     <t>Item-Parent</t>
   </si>
   <si>
@@ -487,6 +504,15 @@
   </si>
   <si>
     <t>Merch List</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>Lighting</t>
+  </si>
+  <si>
+    <t>WE Lighting Fall 2020</t>
   </si>
   <si>
     <t>AttributeName</t>
@@ -1006,9 +1032,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1054,16 +1080,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1093,10 +1112,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1105,14 +1140,6 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1139,9 +1166,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1161,8 +1187,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1175,9 +1202,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1185,21 +1226,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1232,6 +1258,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
       </patternFill>
@@ -1250,49 +1282,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1304,19 +1300,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,6 +1330,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1346,13 +1348,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1376,7 +1372,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1388,19 +1396,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1418,18 +1426,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1462,6 +1488,94 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1473,6 +1587,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1503,24 +1626,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1539,162 +1658,118 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1706,8 +1781,32 @@
     <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1731,15 +1830,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1"/>
@@ -2208,7 +2315,7 @@
       <c r="V2" s="12">
         <v>60</v>
       </c>
-      <c r="AM2" s="17" t="s">
+      <c r="AM2" s="25" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2279,7 +2386,7 @@
       <c r="V3" s="12">
         <v>60</v>
       </c>
-      <c r="AM3" s="17" t="s">
+      <c r="AM3" s="25" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2625,126 +2732,126 @@
       <c r="V8" s="12">
         <v>60</v>
       </c>
-      <c r="AM8" s="17" t="s">
+      <c r="AM8" s="25" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" ht="12.5" spans="1:39">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="16" t="s">
+      <c r="F9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" s="16">
+      <c r="I9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="24">
         <v>50</v>
       </c>
-      <c r="O9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="T9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="U9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="V9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="W9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="X9" s="16" t="s">
+      <c r="O9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="R9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="T9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="U9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="V9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="W9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="X9" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="Y9" s="16" t="s">
+      <c r="Y9" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK9" s="18" t="s">
+      <c r="Z9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK9" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="AL9" s="18" t="s">
+      <c r="AL9" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="AM9" s="16"/>
+      <c r="AM9" s="24"/>
     </row>
     <row r="10" ht="12.5" spans="1:39">
       <c r="A10" s="12" t="s">
@@ -2789,31 +2896,31 @@
       <c r="N10" s="12">
         <v>50</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="O10" s="28" t="s">
         <v>73</v>
       </c>
       <c r="P10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Q10" s="20" t="s">
+      <c r="Q10" s="28" t="s">
         <v>73</v>
       </c>
       <c r="R10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="T10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W10" s="20" t="s">
+      <c r="S10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W10" s="28" t="s">
         <v>73</v>
       </c>
       <c r="X10" s="12" t="s">
@@ -2825,40 +2932,40 @@
       <c r="Z10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AA10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK10" s="17" t="s">
+      <c r="AA10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ10" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK10" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="AL10" s="17" t="s">
+      <c r="AL10" s="25" t="s">
         <v>76</v>
       </c>
       <c r="AM10" s="12"/>
@@ -2912,64 +3019,64 @@
       <c r="P11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="Q11" s="23">
         <v>43891</v>
       </c>
       <c r="R11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="T11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y11" s="20" t="s">
+      <c r="S11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y11" s="28" t="s">
         <v>73</v>
       </c>
       <c r="Z11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AA11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ11" s="20" t="s">
+      <c r="AA11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ11" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AK11" s="12"/>
@@ -3034,22 +3141,22 @@
       <c r="S12" s="12">
         <v>55</v>
       </c>
-      <c r="T12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y12" s="20" t="s">
+      <c r="T12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y12" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AA12" s="12">
@@ -3064,22 +3171,22 @@
       <c r="AD12" s="12">
         <v>2</v>
       </c>
-      <c r="AE12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ12" s="20" t="s">
+      <c r="AE12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ12" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AK12" s="12"/>
@@ -3144,25 +3251,25 @@
       <c r="S13" s="12">
         <v>55</v>
       </c>
-      <c r="T13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z13" s="20" t="s">
+      <c r="T13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z13" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AA13" s="12">
@@ -3177,22 +3284,22 @@
       <c r="AD13" s="12">
         <v>2</v>
       </c>
-      <c r="AE13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ13" s="20" t="s">
+      <c r="AE13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ13" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AK13" s="12"/>
@@ -3254,28 +3361,28 @@
       <c r="R14" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="T14" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="V14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="W14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="X14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z14" s="21" t="s">
+      <c r="S14" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T14" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="V14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="W14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="X14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z14" s="29" t="s">
         <v>73</v>
       </c>
       <c r="AA14">
@@ -3293,19 +3400,19 @@
       <c r="AE14" t="s">
         <v>95</v>
       </c>
-      <c r="AF14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI14" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ14" s="21" t="s">
+      <c r="AF14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ14" s="29" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3364,58 +3471,58 @@
       <c r="R15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="T15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ15" s="20" t="s">
+      <c r="S15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ15" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AK15" s="12"/>
@@ -3465,70 +3572,70 @@
       <c r="N16" s="12">
         <v>50</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="28" t="s">
         <v>73</v>
       </c>
       <c r="P16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Q16" s="20" t="s">
+      <c r="Q16" s="28" t="s">
         <v>73</v>
       </c>
       <c r="R16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="T16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y16" s="20" t="s">
+      <c r="S16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y16" s="28" t="s">
         <v>73</v>
       </c>
       <c r="Z16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AA16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE16" s="20" t="s">
+      <c r="AA16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE16" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AF16" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="AG16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ16" s="20" t="s">
+      <c r="AG16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ16" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AK16" s="12"/>
@@ -3578,7 +3685,7 @@
       <c r="N17" s="12">
         <v>50</v>
       </c>
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="28" t="s">
         <v>73</v>
       </c>
       <c r="P17" s="12" t="s">
@@ -3590,58 +3697,58 @@
       <c r="R17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="T17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y17" s="20" t="s">
+      <c r="S17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y17" s="28" t="s">
         <v>73</v>
       </c>
       <c r="Z17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AA17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG17" s="17" t="s">
+      <c r="AA17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG17" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="AH17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ17" s="20" t="s">
+      <c r="AH17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ17" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AK17" s="12"/>
@@ -3691,7 +3798,7 @@
       <c r="N18" s="12">
         <v>50</v>
       </c>
-      <c r="O18" s="20" t="s">
+      <c r="O18" s="28" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="12" t="s">
@@ -3706,55 +3813,55 @@
       <c r="S18" s="12">
         <v>55</v>
       </c>
-      <c r="T18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="U18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y18" s="20" t="s">
+      <c r="T18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="U18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y18" s="28" t="s">
         <v>73</v>
       </c>
       <c r="Z18" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AA18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ18" s="20" t="s">
+      <c r="AA18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ18" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AK18" s="12"/>
@@ -3807,7 +3914,7 @@
       <c r="P19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Q19" s="20" t="s">
+      <c r="Q19" s="28" t="s">
         <v>73</v>
       </c>
       <c r="R19" s="12" t="s">
@@ -3819,43 +3926,43 @@
       <c r="T19" s="12">
         <v>62</v>
       </c>
-      <c r="U19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="V19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="W19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="X19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y19" s="20" t="s">
+      <c r="U19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="V19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y19" s="28" t="s">
         <v>73</v>
       </c>
       <c r="Z19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AA19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG19" s="20" t="s">
+      <c r="AA19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG19" s="28" t="s">
         <v>73</v>
       </c>
       <c r="AH19" s="12" t="s">
@@ -3962,16 +4069,16 @@
       <c r="D2" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="23">
         <v>45292</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="23">
         <v>45293</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="23">
         <v>45292</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="23">
         <v>45293</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -3983,16 +4090,16 @@
       <c r="K2" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="23">
         <v>45293</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="23">
         <v>45294</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2" s="23">
         <v>45294</v>
       </c>
-      <c r="O2" s="15">
+      <c r="O2" s="23">
         <v>45295</v>
       </c>
     </row>
@@ -4009,16 +4116,16 @@
       <c r="D3" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="23">
         <v>45659</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="23">
         <v>45845</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="23">
         <v>45999</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="23">
         <v>46019</v>
       </c>
       <c r="I3" s="12" t="s">
@@ -4030,16 +4137,16 @@
       <c r="K3" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="23">
         <v>45691</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="23">
         <v>45846</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="23">
         <v>45999</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="23">
         <v>46019</v>
       </c>
     </row>
@@ -4054,110 +4161,226 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="20.7090909090909" customWidth="1"/>
+    <col min="4" max="4" width="20.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13" spans="1:1">
-      <c r="A1" s="9" t="s">
+    <row r="1" ht="13.75" spans="1:4">
+      <c r="A1" s="15" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" ht="12.5" spans="1:1">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" ht="12.5" spans="1:1">
-      <c r="A3" s="12" t="s">
+      <c r="D1" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" ht="12.5" spans="1:4">
+      <c r="A2" s="18" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" ht="12.5" spans="1:1">
-      <c r="A4" s="12" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" ht="12.5" spans="1:4">
+      <c r="A3" s="20" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="5" ht="12.5" spans="1:1">
-      <c r="A5" s="12" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" ht="12.5" spans="1:4">
+      <c r="A4" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" ht="12.5" spans="1:4">
+      <c r="A5" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" ht="12.5" spans="1:4">
+      <c r="A6" s="20" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" ht="12.5" spans="1:1">
-      <c r="A6" s="12" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" ht="12.5" spans="1:4">
+      <c r="A7" s="20" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" ht="12.5" spans="1:1">
-      <c r="A7" s="12" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:4">
+      <c r="A8" s="21" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="8" ht="12.5" spans="1:1">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" ht="12.5" spans="1:4">
+      <c r="A9" s="20" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="9" ht="12.5" spans="1:1">
-      <c r="A9" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" ht="12.5" spans="1:1">
-      <c r="A10" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" ht="12.5" spans="1:1">
-      <c r="A11" s="12" t="s">
+      <c r="B9" s="21" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" ht="12.5" spans="1:1">
-      <c r="A12" s="12" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" ht="12.5" spans="1:4">
+      <c r="A10" s="20" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="13" ht="12.5" spans="1:1">
-      <c r="A13" s="12" t="s">
+      <c r="B10" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" ht="12.5" spans="1:4">
+      <c r="A11" s="20" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="14" ht="12.5" spans="1:1">
-      <c r="A14" s="12" t="s">
+      <c r="B11" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:4">
+      <c r="A12" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:4">
+      <c r="A13" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" ht="12.5" spans="1:4">
+      <c r="A14" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" ht="12.5" spans="1:4">
+      <c r="A15" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" ht="12.5" spans="1:4">
+      <c r="A16" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" ht="12.5" spans="1:4">
+      <c r="A17" s="20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" ht="12.5" spans="1:1">
-      <c r="A15" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" ht="12.5" spans="1:1">
-      <c r="A16" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" ht="12.5" spans="1:1">
-      <c r="A17" s="12" t="s">
+      <c r="B17" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="18" ht="12.5" spans="1:1">
-      <c r="A18" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" ht="12.5" spans="1:1">
-      <c r="A19" s="12" t="s">
-        <v>155</v>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" ht="12.5" spans="1:4">
+      <c r="A18" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" ht="12.5" spans="1:4">
+      <c r="A19" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" ht="12.5" spans="1:4">
+      <c r="A20" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4167,123 +4390,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:A19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="20.7090909090909" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="13" spans="1:1">
-      <c r="A1" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" ht="12.5" spans="1:1">
-      <c r="A2" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" ht="12.5" spans="1:1">
-      <c r="A3" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" ht="12.5" spans="1:1">
-      <c r="A4" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" ht="12.5" spans="1:1">
-      <c r="A5" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" ht="12.5" spans="1:1">
-      <c r="A6" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" ht="12.5" spans="1:1">
-      <c r="A7" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" ht="12.5" spans="1:1">
-      <c r="A8" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" ht="12.5" spans="1:1">
-      <c r="A9" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" ht="12.5" spans="1:1">
-      <c r="A10" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" ht="12.5" spans="1:1">
-      <c r="A11" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" ht="12.5" spans="1:1">
-      <c r="A12" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" ht="12.5" spans="1:1">
-      <c r="A13" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" ht="12.5" spans="1:1">
-      <c r="A14" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" ht="12.5" spans="1:1">
-      <c r="A15" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" ht="12.5" spans="1:1">
-      <c r="A16" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" ht="12.5" spans="1:1">
-      <c r="A17" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" ht="12.5" spans="1:1">
-      <c r="A18" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" ht="12.5" spans="1:1">
-      <c r="A19" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D13"/>
@@ -4303,13 +4409,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4320,10 +4426,10 @@
         <v>117</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4334,10 +4440,10 @@
         <v>117</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4348,7 +4454,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>132</v>
@@ -4362,7 +4468,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>131</v>
@@ -4373,10 +4479,10 @@
         <v>53</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>130</v>
@@ -4387,13 +4493,13 @@
         <v>53</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4401,12 +4507,12 @@
         <v>53</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D8" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4415,13 +4521,13 @@
         <v>81</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4429,13 +4535,13 @@
         <v>81</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4443,13 +4549,13 @@
         <v>81</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4457,13 +4563,13 @@
         <v>81</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4471,12 +4577,12 @@
         <v>81</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D13" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4486,12 +4592,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -4506,25 +4612,25 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" ht="50" spans="1:8">
@@ -4532,13 +4638,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="E2" s="6" t="str">
         <f t="shared" ref="E2:E65" si="0">_xlfn.CONCAT(C2,D2)</f>
@@ -4553,7 +4659,7 @@
         <v>tstvcaweba@wsgc.com</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" ht="50" spans="1:8">
@@ -4561,13 +4667,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E3" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4582,7 +4688,7 @@
         <v>tstvcapbba@wsgc.com</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" ht="50" spans="1:8">
@@ -4590,13 +4696,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="E4" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4611,7 +4717,7 @@
         <v>tstvcapkba@wsgc.com</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" ht="50" spans="1:8">
@@ -4619,13 +4725,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="E5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4640,21 +4746,21 @@
         <v>tstvcaptba@wsgc.com</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" ht="37.5" spans="1:8">
       <c r="A6" s="4">
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4669,7 +4775,7 @@
         <v>tstvcawedabm@wsgc.com</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" ht="50" spans="1:8">
@@ -4677,13 +4783,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4698,21 +4804,21 @@
         <v>tstvcawefbm@wsgc.com</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" ht="37.5" spans="1:8">
       <c r="A8" s="4">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4727,21 +4833,21 @@
         <v>tstvcawelbm@wsgc.com</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" ht="37.5" spans="1:8">
       <c r="A9" s="4">
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="E9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4756,21 +4862,21 @@
         <v>tstvcawetbm@wsgc.com</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" ht="37.5" spans="1:8">
       <c r="A10" s="4">
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="E10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4785,7 +4891,7 @@
         <v>tstvcapbdabm@wsgc.com</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" ht="50" spans="1:8">
@@ -4793,13 +4899,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="E11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4814,21 +4920,21 @@
         <v>tstvcapbfbm@wsgc.com</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" ht="37.5" spans="1:8">
       <c r="A12" s="4">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E12" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4843,7 +4949,7 @@
         <v>tstvcapblbm@wsgc.com</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" ht="50" spans="1:8">
@@ -4851,13 +4957,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="E13" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4872,21 +4978,21 @@
         <v>tstvcapbttbm@wsgc.com</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" ht="37.5" spans="1:8">
       <c r="A14" s="4">
         <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4901,21 +5007,21 @@
         <v>tstvcapbtbm@wsgc.com</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" ht="37.5" spans="1:8">
       <c r="A15" s="4">
         <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4930,7 +5036,7 @@
         <v>tstvcapkdabm@wsgc.com</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" ht="50" spans="1:8">
@@ -4938,13 +5044,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4959,21 +5065,21 @@
         <v>tstvcapkfbm@wsgc.com</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" ht="37.5" spans="1:8">
       <c r="A17" s="4">
         <v>17</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4988,21 +5094,21 @@
         <v>tstvcapklbm@wsgc.com</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" ht="37.5" spans="1:8">
       <c r="A18" s="4">
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5017,21 +5123,21 @@
         <v>tstvcapktbm@wsgc.com</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" ht="37.5" spans="1:8">
       <c r="A19" s="4">
         <v>19</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5046,7 +5152,7 @@
         <v>tstvcaptdabm@wsgc.com</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" ht="50" spans="1:8">
@@ -5054,13 +5160,13 @@
         <v>20</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="E20" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5075,21 +5181,21 @@
         <v>tstvcaptfbm@wsgc.com</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="21" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" ht="37.5" spans="1:8">
       <c r="A21" s="4">
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5104,21 +5210,21 @@
         <v>tstvcaptlbm@wsgc.com</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" ht="37.5" spans="1:8">
       <c r="A22" s="4">
         <v>22</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5133,21 +5239,21 @@
         <v>tstvcapttbm@wsgc.com</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="23" ht="25" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" ht="14.5" spans="1:8">
       <c r="A23" s="4">
         <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5162,21 +5268,21 @@
         <v>tstvcamerchops@wsgc.com</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" ht="37.5" spans="1:8">
       <c r="A24" s="4">
         <v>24</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5191,7 +5297,7 @@
         <v>tstvcawedaecm@wsgc.com</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" ht="50" spans="1:8">
@@ -5199,13 +5305,13 @@
         <v>25</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5220,21 +5326,21 @@
         <v>tstvcawefecm@wsgc.com</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="26" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" ht="37.5" spans="1:8">
       <c r="A26" s="4">
         <v>26</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5249,21 +5355,21 @@
         <v>tstvcawelecm@wsgc.com</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" ht="37.5" spans="1:8">
       <c r="A27" s="4">
         <v>27</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5278,21 +5384,21 @@
         <v>tstvcawetecm@wsgc.com</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" ht="37.5" spans="1:8">
       <c r="A28" s="4">
         <v>28</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5307,7 +5413,7 @@
         <v>tstvcapbdaecm@wsgc.com</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" ht="50" spans="1:8">
@@ -5315,13 +5421,13 @@
         <v>29</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5336,21 +5442,21 @@
         <v>tstvcapbfecm@wsgc.com</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" ht="37.5" spans="1:8">
       <c r="A30" s="4">
         <v>30</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5365,7 +5471,7 @@
         <v>tstvcapblecm@wsgc.com</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" ht="50" spans="1:8">
@@ -5373,13 +5479,13 @@
         <v>31</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="E31" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5394,21 +5500,21 @@
         <v>tstvcapbttecm@wsgc.com</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="32" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" ht="37.5" spans="1:8">
       <c r="A32" s="4">
         <v>32</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="E32" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5423,21 +5529,21 @@
         <v>tstvcapbtecm@wsgc.com</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="33" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" ht="37.5" spans="1:8">
       <c r="A33" s="4">
         <v>33</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="E33" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5452,7 +5558,7 @@
         <v>tstvcapkdaecm@wsgc.com</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" ht="50" spans="1:8">
@@ -5460,13 +5566,13 @@
         <v>34</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="E34" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5481,21 +5587,21 @@
         <v>tstvcapkfecm@wsgc.com</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="35" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" ht="37.5" spans="1:8">
       <c r="A35" s="4">
         <v>35</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="E35" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5510,21 +5616,21 @@
         <v>tstvcapklecm@wsgc.com</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="36" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" ht="37.5" spans="1:8">
       <c r="A36" s="4">
         <v>36</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="E36" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5539,21 +5645,21 @@
         <v>tstvcapktecm@wsgc.com</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="37" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" ht="37.5" spans="1:8">
       <c r="A37" s="4">
         <v>37</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="E37" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5568,7 +5674,7 @@
         <v>tstvcaptdaecm@wsgc.com</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" ht="50" spans="1:8">
@@ -5576,13 +5682,13 @@
         <v>38</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="E38" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5597,21 +5703,21 @@
         <v>tstvcaptfecm@wsgc.com</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" ht="37.5" spans="1:8">
       <c r="A39" s="4">
         <v>39</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E39" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5626,21 +5732,21 @@
         <v>tstvcaptlecm@wsgc.com</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="40" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" ht="37.5" spans="1:8">
       <c r="A40" s="4">
         <v>40</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="E40" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5655,7 +5761,7 @@
         <v>tstvcapttecm@wsgc.com</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" ht="37.5" spans="1:8">
@@ -5663,13 +5769,13 @@
         <v>41</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="E41" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5684,21 +5790,21 @@
         <v>tstvcawelifem@wsgc.com</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" ht="37.5" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" ht="25" spans="1:8">
       <c r="A42" s="4">
         <v>42</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="E42" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5713,21 +5819,21 @@
         <v>tstvcapblifem@wsgc.com</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="43" ht="37.5" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" ht="25" spans="1:8">
       <c r="A43" s="4">
         <v>43</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="E43" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5742,21 +5848,21 @@
         <v>tstvcapklifem@wsgc.com</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="44" ht="37.5" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" ht="25" spans="1:8">
       <c r="A44" s="4">
         <v>44</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="E44" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5771,21 +5877,21 @@
         <v>tstvcaptlifem@wsgc.com</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" ht="50" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" ht="37.5" spans="1:8">
       <c r="A45" s="4">
         <v>45</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="E45" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5800,7 +5906,7 @@
         <v>tstvcawedsp@wsgc.com</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" ht="37.5" spans="1:8">
@@ -5808,13 +5914,13 @@
         <v>46</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="E46" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5829,7 +5935,7 @@
         <v>tstvcapbdsp@wsgc.com</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" ht="37.5" spans="1:8">
@@ -5837,13 +5943,13 @@
         <v>47</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="E47" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5858,7 +5964,7 @@
         <v>tstvcaptdsp@wsgc.com</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" ht="37.5" spans="1:8">
@@ -5866,13 +5972,13 @@
         <v>48</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="E48" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5887,7 +5993,7 @@
         <v>tstvcapkdsp@wsgc.com</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" ht="37.5" spans="1:8">
@@ -5895,13 +6001,13 @@
         <v>49</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="E49" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5916,7 +6022,7 @@
         <v>tstvcawesm@wsgc.com</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" ht="37.5" spans="1:8">
@@ -5924,13 +6030,13 @@
         <v>50</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="E50" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5945,7 +6051,7 @@
         <v>tstvcapbsm@wsgc.com</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" ht="37.5" spans="1:8">
@@ -5953,13 +6059,13 @@
         <v>51</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="E51" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5974,21 +6080,21 @@
         <v>tstvcapksm@wsgc.com</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="52" ht="37.5" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" ht="25" spans="1:8">
       <c r="A52" s="4">
         <v>52</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="E52" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6003,7 +6109,7 @@
         <v>tstvcaptsm@wsgc.com</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" ht="37.5" spans="1:8">
@@ -6011,13 +6117,13 @@
         <v>53</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="E53" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6032,7 +6138,7 @@
         <v>tstvcaweim@wsgc.com</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" ht="37.5" spans="1:8">
@@ -6040,13 +6146,13 @@
         <v>54</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="E54" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6061,7 +6167,7 @@
         <v>tstvcapbim@wsgc.com</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" ht="37.5" spans="1:8">
@@ -6069,13 +6175,13 @@
         <v>55</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="E55" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6090,7 +6196,7 @@
         <v>tstvcapkim@wsgc.com</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" ht="37.5" spans="1:8">
@@ -6098,13 +6204,13 @@
         <v>56</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="E56" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6119,21 +6225,21 @@
         <v>tstvcaptim@wsgc.com</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="57" ht="37.5" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" ht="25" spans="1:8">
       <c r="A57" s="4">
         <v>57</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="E57" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6148,7 +6254,7 @@
         <v>tstvcawegbm@wsgc.com</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" ht="25" spans="1:8">
@@ -6156,13 +6262,13 @@
         <v>58</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E58" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6177,7 +6283,7 @@
         <v>tstvcapbgbm@wsgc.com</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" ht="25" spans="1:8">
@@ -6185,13 +6291,13 @@
         <v>59</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="E59" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6206,7 +6312,7 @@
         <v>tstvcapkgbm@wsgc.com</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" ht="25" spans="1:8">
@@ -6214,13 +6320,13 @@
         <v>60</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="E60" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6235,7 +6341,7 @@
         <v>tstvcaptgbm@wsgc.com</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" ht="37.5" spans="1:8">
@@ -6243,13 +6349,13 @@
         <v>61</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="E61" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6264,7 +6370,7 @@
         <v>tstvcawebanalyst@wsgc.com</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" ht="37.5" spans="1:8">
@@ -6272,13 +6378,13 @@
         <v>62</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="E62" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6293,7 +6399,7 @@
         <v>tstvcapbbanalyst@wsgc.com</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" ht="37.5" spans="1:8">
@@ -6301,13 +6407,13 @@
         <v>63</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="E63" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6322,7 +6428,7 @@
         <v>tstvcapkbanalyst@wsgc.com</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="64" ht="37.5" spans="1:8">
@@ -6330,13 +6436,13 @@
         <v>64</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="E64" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6351,21 +6457,21 @@
         <v>tstvcaptbanalyst@wsgc.com</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="65" ht="25" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" ht="14.5" spans="1:8">
       <c r="A65" s="4">
         <v>65</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="E65" s="6" t="str">
         <f t="shared" si="0"/>
@@ -6380,7 +6486,7 @@
         <v>tstvcaweguest@wsgc.com</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" ht="14.5" spans="1:8">
@@ -6388,13 +6494,13 @@
         <v>66</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="E66" s="6" t="str">
         <f t="shared" ref="E66:E68" si="3">_xlfn.CONCAT(C66,D66)</f>
@@ -6409,7 +6515,7 @@
         <v>tstvcapbguest@wsgc.com</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" ht="14.5" spans="1:8">
@@ -6417,13 +6523,13 @@
         <v>67</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="E67" s="6" t="str">
         <f t="shared" si="3"/>
@@ -6438,7 +6544,7 @@
         <v>tstvcapkguest@wsgc.com</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" ht="14.5" spans="1:8">
@@ -6446,13 +6552,13 @@
         <v>68</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="E68" s="6" t="str">
         <f t="shared" si="3"/>
@@ -6467,7 +6573,7 @@
         <v>tstvcaptguest@wsgc.com</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>